<commit_message>
Converti para json gerado do Excel. Actualizei tabelas do Continente.
</commit_message>
<xml_diff>
--- a/FlatTaxPT.ExtracaoTabelas/TabelasRetencao.xlsx
+++ b/FlatTaxPT.ExtracaoTabelas/TabelasRetencao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psampaio\Projects\FlatTaxPT\FlatTaxPT.ExtracaoTabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7785F8-A5D8-4BAA-AA88-A010449A338A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6D50AE-3D07-4CF7-A988-A4E06668D5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Dependente_NaoCasado">Continente!$A$3:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,25 +30,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Dependente Não Casado</t>
-  </si>
-  <si>
     <t>Remuneração</t>
   </si>
   <si>
-    <t>Dependente Casado Único</t>
+    <t>Dependente NaoCasado</t>
   </si>
   <si>
-    <t>Dependente Casado Dois</t>
+    <t>Dependente CasadoUnico</t>
   </si>
   <si>
-    <t>Dependente Não Casado Deficiente</t>
+    <t>Dependente CasadoDois</t>
   </si>
   <si>
-    <t>Dependente Casado Único Deficiente</t>
+    <t>Dependente NaoCasado Deficiente</t>
   </si>
   <si>
-    <t>Dependente Casado Dois Deficiente</t>
+    <t>Dependente CasadoUnico Deficiente</t>
+  </si>
+  <si>
+    <t>Dependente CasadoDois Deficiente</t>
   </si>
 </sst>
 </file>
@@ -56,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -104,8 +104,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -393,7 +393,7 @@
   <dimension ref="A1:AK38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +404,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -454,7 +454,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>

</xml_diff>